<commit_message>
Agent query: Por favor, verifica si: 1) Los botones de exportación están visibles 2) Se pueden exportar los datos a Excel y CSV 3) Los archivos se pueden descargar correctamente
</commit_message>
<xml_diff>
--- a/datos_ine.xlsx
+++ b/datos_ine.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -472,13 +472,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>648</v>
+        <v>760</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -492,13 +492,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>634</v>
+        <v>739</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,13 +512,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>632</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -532,18 +532,18 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>647</v>
+        <v>761</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>HOMBRE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -552,18 +552,18 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>355</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>HOMBRE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -572,18 +572,18 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>343</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>HOMBRE</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -592,18 +592,18 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>344</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>HOMBRE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -612,18 +612,18 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>350</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>MUJER</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -632,18 +632,18 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>293</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>MUJER</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -652,18 +652,18 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>291</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>MUJER</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -672,18 +672,18 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>288</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Alcadozo</t>
+          <t>Abengibre</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>MUJER</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>297</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>